<commit_message>
added SSOC assigner, 2024 detailed definitions
</commit_message>
<xml_diff>
--- a/output/CLFS_sample_input_validation_report.xlsx
+++ b/output/CLFS_sample_input_validation_report.xlsx
@@ -414,7 +414,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D5"/>
+  <dimension ref="A1:D6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -507,20 +507,40 @@
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
+          <t>RULE 10</t>
+        </is>
+      </c>
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>Was your main job last week a paid internship, traineeship or apprenticeship? &amp; Type of Employment?</t>
+        </is>
+      </c>
+      <c r="C5" t="inlineStr">
+        <is>
+          <t>Internship/Traineeship/Apprenticeship must be Fixed-Term contract employee</t>
+        </is>
+      </c>
+      <c r="D5" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="inlineStr">
+        <is>
           <t>RULE 5</t>
         </is>
       </c>
-      <c r="B5" t="inlineStr">
+      <c r="B6" t="inlineStr">
         <is>
           <t>How much interest did you receive from savings (e.g., current and saving accounts, fixed deposits) in the last 12 months?</t>
         </is>
       </c>
-      <c r="C5" t="inlineStr">
+      <c r="C6" t="inlineStr">
         <is>
           <t>Invalid interest. Must be numeric between 0 and 10 (decimals allowed).</t>
         </is>
       </c>
-      <c r="D5" t="n">
+      <c r="D6" t="n">
         <v>1</v>
       </c>
     </row>
@@ -535,7 +555,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:H7"/>
+  <dimension ref="A1:H8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -807,6 +827,44 @@
         </is>
       </c>
     </row>
+    <row r="8">
+      <c r="A8" t="inlineStr">
+        <is>
+          <t>CLFS_sample_input.xlsx</t>
+        </is>
+      </c>
+      <c r="B8" t="n">
+        <v>4</v>
+      </c>
+      <c r="C8" t="inlineStr">
+        <is>
+          <t>697c2c580deae81fbb49c180</t>
+        </is>
+      </c>
+      <c r="D8" t="n">
+        <v>1</v>
+      </c>
+      <c r="E8" t="inlineStr">
+        <is>
+          <t>Chen Jia Hui</t>
+        </is>
+      </c>
+      <c r="F8" t="inlineStr">
+        <is>
+          <t>RULE 10</t>
+        </is>
+      </c>
+      <c r="G8" t="inlineStr">
+        <is>
+          <t>Was your main job last week a paid internship, traineeship or apprenticeship? &amp; Type of Employment?</t>
+        </is>
+      </c>
+      <c r="H8" t="inlineStr">
+        <is>
+          <t>Internship/Traineeship/Apprenticeship must be Fixed-Term contract employee</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>